<commit_message>
added 2 lead test case, added pageobject manager
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/data.xlsx
+++ b/src/test/resources/TestData/data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CE34BA-3CBB-4691-9B76-3700D45B296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>TCName</t>
   </si>
@@ -73,13 +74,67 @@
   </si>
   <si>
     <t>vtiger CRM - Commercial Open Source CRM</t>
+  </si>
+  <si>
+    <t>TC06_CreateLeadWithMandatoryFields</t>
+  </si>
+  <si>
+    <t>TC07_EditLead_DeleteLead</t>
+  </si>
+  <si>
+    <t>Last Name cannot be empty</t>
+  </si>
+  <si>
+    <t>ExpAlert1</t>
+  </si>
+  <si>
+    <t>Lead Source</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>EmailWrong</t>
+  </si>
+  <si>
+    <t>EmailRight</t>
+  </si>
+  <si>
+    <t>hgdhjw</t>
+  </si>
+  <si>
+    <t>ddhg@gmail.com</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>No of employees</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Lead Status</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Please enter a valid Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +146,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,25 +188,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +258,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -209,6 +292,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -243,9 +327,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,20 +503,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,10 +543,38 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -464,11 +584,11 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="O2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -479,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -490,7 +610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -501,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -521,31 +641,101 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
+      <c r="I8">
+        <v>776127892</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M8" r:id="rId1" xr:uid="{E90ED5E9-4498-401D-A637-1ABF18BDF973}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>